<commit_message>
updated the profiles ctdc qa and dev.  troubleshooting db connection
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
+++ b/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD91B467-48B2-4B34-8F5B-D4F7A02134EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E07596A-12C1-4D89-AC1F-55EC2B1CA79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.gender IN ['FEMALE']  OPTIONAL MATCH (s)&lt;-[*]-(f:file) RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>Cases</t>
   </si>
 </sst>
 </file>
@@ -424,44 +430,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.81640625" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the contents of tabname in input excel for CTDC
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
+++ b/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E07596A-12C1-4D89-AC1F-55EC2B1CA79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A675B97-5748-4EF7-8544-635B021CB9D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -60,7 +60,7 @@
     <t>TabName</t>
   </si>
   <si>
-    <t>Cases</t>
+    <t>CasesTab</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated ctdc dev queries
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
+++ b/InputFiles/TC02_Trials_Filter_Gender-Female.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A675B97-5748-4EF7-8544-635B021CB9D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3DEF42-D999-45EC-BCDB-73CF7C131259}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -48,19 +48,36 @@
     <t>TC02_Trials_Filter_Gender-Female_WebData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.gender IN ['FEMALE'] RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(t.clinical_trial_designation ,'')as `Trial Code` , coalesce(a.arm_id,'') As `Arm` , coalesce(a.arm_drug,'') As `Arm Treatment` , coalesce(c.disease,'') As Diagnosis , coalesce(c.gender,'') As Gender , coalesce(c.race,'') As Race , coalesce(c.ethnicity,'') As Ethnicity</t>
-  </si>
-  <si>
     <t>StatQuery</t>
   </si>
   <si>
-    <t>MATCH (t:clinical_trial)&lt;--(a:arm)&lt;--(c:case)&lt;--(s:specimen)&lt;--(:assignment_report) WITH DISTINCT c AS c, t ,a, s WHERE c.gender IN ['FEMALE']  OPTIONAL MATCH (s)&lt;-[*]-(f:file) RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(t.clinical_trial_designation)) as number_of_trial</t>
-  </si>
-  <si>
     <t>TabName</t>
   </si>
   <si>
     <t>CasesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)
+    WHERE c.gender = "FEMALE"
+WITH DISTINCT c, a, ct
+RETURN 
+    COALESCE(c.case_id, '') AS `Case ID`,
+    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
+    COALESCE(a.arm_id, '') AS `Arm`,
+    COALESCE(a.arm_drug, '') AS `Arm Treatment`,
+    COALESCE(c.disease, '') AS `Diagnosis`,
+    COALESCE(c.gender, '') AS `Gender`,
+    COALESCE(c.race, '') AS `Race`,
+    COALESCE(c.ethnicity, '') AS `Ethnicity`</t>
+  </si>
+  <si>
+    <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(:arm)--&gt;(ct:clinical_trial)
+    WHERE c.gender = "FEMALE"
+OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
+RETURN 
+    COUNT(DISTINCT f) AS number_of_files,
+    COUNT(DISTINCT c.case_id) AS number_of_cases,
+    COUNT(DISTINCT ct.clinical_trial_designation) AS number_of_trials</t>
   </si>
 </sst>
 </file>
@@ -433,7 +450,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,13 +463,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -461,15 +478,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>

</xml_diff>